<commit_message>
excel adjustment-> gas in m3pa instead of kWhpa
</commit_message>
<xml_diff>
--- a/data_ProjectTemplate/Buildings_ProjectTemplate.xlsx
+++ b/data_ProjectTemplate/Buildings_ProjectTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\LUX_ProjectTemplate\data_ProjectTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99510529-5A2C-4120-84AF-4EC5ADE37644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13149339-643D-44BF-BF53-D5A0B0256AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{99A50208-934F-4EDD-BF51-6D238E9C57FC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{99A50208-934F-4EDD-BF51-6D238E9C57FC}"/>
   </bookViews>
   <sheets>
     <sheet name="buildings" sheetId="4" r:id="rId1"/>
@@ -684,9 +684,6 @@
     <t>energy_label</t>
   </si>
   <si>
-    <t>gas_consumption_kwhpa</t>
-  </si>
-  <si>
     <t>electricity_consumption_kwhpa</t>
   </si>
   <si>
@@ -742,6 +739,9 @@
   </si>
   <si>
     <t>address_floor_surface_m2</t>
+  </si>
+  <si>
+    <t>gas_consumption_m3pa</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD9D70-6DEB-4390-947E-55D38CEBDCD5}">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1170,7 +1170,7 @@
     <col min="16" max="16" width="91.08984375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.81640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
@@ -1179,67 +1179,67 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>2</v>

</xml_diff>